<commit_message>
Adding chat windows and updating diagrams with chat function
</commit_message>
<xml_diff>
--- a/doc/userstory/userstory.xlsx
+++ b/doc/userstory/userstory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5557799d0b7a6a6f/bsc-thesis/doc/userstory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="267" documentId="8_{834A9F3F-811A-48FA-97A4-966026AC1D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF64CE99-630A-414F-BB2F-94AB13DC8DF4}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{834A9F3F-811A-48FA-97A4-966026AC1D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD7CFBA3-F60A-4BE5-B273-955898AC42E7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{2B397BC3-7B9C-4148-B77D-4D3251D00AB4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="121">
   <si>
     <t>GIVEN</t>
   </si>
@@ -378,6 +378,27 @@
   </si>
   <si>
     <t>Kilistázásra kerülnek a megfelelő ligák/csapatok, mint linkek</t>
+  </si>
+  <si>
+    <t>Chatelés más emberekkel adott meccsről</t>
+  </si>
+  <si>
+    <t>Adott mérkőzéshez tartozó oldalon</t>
+  </si>
+  <si>
+    <t>Az üzenet elmentésre kerül a szerveren, amit mindenki más láthat a megfelelő chatablakban</t>
+  </si>
+  <si>
+    <t>Chatelés a résztvevőkkel</t>
+  </si>
+  <si>
+    <t>Beírok egy üzenetet, és elküldöm</t>
+  </si>
+  <si>
+    <t>Az üzenet elmentésre kerül a szerveren, amit minden más résztvevő is láthat a megfelelő chatablakban</t>
+  </si>
+  <si>
+    <t>Beírok egy üzenetet és elküldöm azt</t>
   </si>
 </sst>
 </file>
@@ -484,16 +505,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF9A114-32E7-479E-BAF0-398ED11E9564}">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:C100"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,16 +876,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -875,7 +896,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -884,7 +905,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -900,7 +921,7 @@
       <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -911,7 +932,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -920,7 +941,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -929,7 +950,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -940,7 +961,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
@@ -949,7 +970,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -958,7 +979,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -969,7 +990,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
@@ -978,7 +999,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -987,7 +1008,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -998,7 +1019,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1028,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1037,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1027,7 +1048,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1057,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1066,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1056,7 +1077,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +1086,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1095,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1085,7 +1106,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1115,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1131,7 @@
       <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1121,7 +1142,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="6"/>
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1130,7 +1151,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="6"/>
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1139,7 +1160,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1150,7 +1171,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1159,7 +1180,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1168,7 +1189,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1179,7 +1200,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="1" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1209,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1197,73 +1218,73 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="2" t="s">
+    <row r="42" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" s="2" t="s">
+    <row r="43" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+    <row r="44" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>0</v>
@@ -1273,120 +1294,120 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="2" t="s">
+    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+    <row r="50" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="2" t="s">
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="2" t="s">
+    <row r="52" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="2" t="s">
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
-      <c r="B53" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="2" t="s">
+    <row r="56" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="5"/>
-      <c r="B55" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
@@ -1396,55 +1417,55 @@
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="5"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
+      <c r="B61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" s="2" t="s">
+    <row r="62" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
-      <c r="B62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>0</v>
@@ -1454,26 +1475,26 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
+      <c r="A64" s="7"/>
       <c r="B64" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A65" s="7"/>
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>72</v>
+      <c r="A66" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>0</v>
@@ -1483,149 +1504,149 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="7"/>
       <c r="B67" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="7"/>
+      <c r="B68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="7"/>
+      <c r="B70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C68" s="2" t="s">
+    <row r="71" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="7"/>
+      <c r="B71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-    </row>
-    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="B73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" s="2" t="s">
+    <row r="74" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="7"/>
+      <c r="B74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" s="2" t="s">
+    <row r="75" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="7"/>
+      <c r="B75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
+    <row r="76" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="2" t="s">
+      <c r="B76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
-      <c r="B74" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C74" s="2" t="s">
+    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="7"/>
+      <c r="B77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
-      <c r="B75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="2" t="s">
+    <row r="78" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A78" s="7"/>
+      <c r="B78" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
+    <row r="79" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="B79" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="5"/>
-      <c r="B77" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C77" s="2" t="s">
+    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="7"/>
+      <c r="B80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="5"/>
-      <c r="B78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="2" t="s">
+    <row r="81" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="7"/>
+      <c r="B81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
+    <row r="82" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
-      <c r="B80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="5"/>
-      <c r="B81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>0</v>
@@ -1635,141 +1656,141 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="5"/>
+      <c r="A83" s="7"/>
       <c r="B83" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="7"/>
+      <c r="B84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="7"/>
+      <c r="B86" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A84" s="5"/>
-      <c r="B84" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" s="2" t="s">
+    <row r="87" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
+    <row r="88" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C85" s="2" t="s">
+      <c r="B88" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="5"/>
-      <c r="B86" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C86" s="2" t="s">
+    <row r="89" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="5"/>
-      <c r="B87" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" s="2" t="s">
+    <row r="90" spans="1:3" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="7"/>
+      <c r="B90" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
+    <row r="91" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="5"/>
-      <c r="B89" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" s="2" t="s">
+    <row r="92" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="7"/>
+      <c r="B92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A90" s="5"/>
-      <c r="B90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="2" t="s">
+    <row r="93" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A93" s="7"/>
+      <c r="B93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
+    <row r="94" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C91" s="2" t="s">
+      <c r="B94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="5"/>
-      <c r="B92" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C92" s="2" t="s">
+    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="7"/>
+      <c r="B95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="5"/>
-      <c r="B93" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93" s="2" t="s">
+    <row r="96" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A96" s="7"/>
+      <c r="B96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="5"/>
-      <c r="B95" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="5"/>
-      <c r="B96" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="97" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -1780,80 +1801,136 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="5"/>
+      <c r="A98" s="7"/>
       <c r="B98" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="7"/>
+      <c r="B99" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="7"/>
+      <c r="B101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A99" s="5"/>
-      <c r="B99" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C99" s="2" t="s">
+    <row r="102" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A102" s="7"/>
+      <c r="B102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="8" t="s">
+    <row r="103" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="7"/>
+      <c r="B104" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A105" s="7"/>
+      <c r="B105" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-    </row>
-    <row r="101" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+    </row>
+    <row r="107" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C101" s="2" t="s">
+      <c r="B107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A102" s="5"/>
-      <c r="B102" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C102" s="2" t="s">
+    <row r="108" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A108" s="7"/>
+      <c r="B108" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A103" s="5"/>
-      <c r="B103" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C103" s="2" t="s">
+    <row r="109" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A109" s="7"/>
+      <c r="B109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:C69"/>
+  <mergeCells count="40">
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A85:A87"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A28:A30"/>
@@ -1862,17 +1939,21 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Countries and leagues API endpoints implemented
</commit_message>
<xml_diff>
--- a/doc/userstory/userstory.xlsx
+++ b/doc/userstory/userstory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5557799d0b7a6a6f/bsc-thesis/doc/userstory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="288" documentId="8_{834A9F3F-811A-48FA-97A4-966026AC1D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD7CFBA3-F60A-4BE5-B273-955898AC42E7}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{834A9F3F-811A-48FA-97A4-966026AC1D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A3A6C2F-BF97-43F6-96A7-E86A2014562C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{2B397BC3-7B9C-4148-B77D-4D3251D00AB4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{2B397BC3-7B9C-4148-B77D-4D3251D00AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -506,7 +506,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -515,9 +515,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -538,10 +535,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF9A114-32E7-479E-BAF0-398ED11E9564}">
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +872,7 @@
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
@@ -914,11 +907,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
@@ -1124,11 +1117,11 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -1247,11 +1240,11 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
@@ -1370,11 +1363,11 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
@@ -1551,11 +1544,11 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
     </row>
     <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
@@ -1877,11 +1870,11 @@
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="8" t="s">
+      <c r="A106" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
     </row>
     <row r="107" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
@@ -1914,19 +1907,15 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="A76:A78"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A91:A93"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A41:A43"/>
@@ -1942,18 +1931,22 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A85:A87"/>
     <mergeCell ref="A73:A75"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>